<commit_message>
study2 and study3 update
</commit_message>
<xml_diff>
--- a/study3/survey_materials/generated_ads_for_survey_study3_final.xlsx
+++ b/study3/survey_materials/generated_ads_for_survey_study3_final.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2d319992da703ee6/Desktop/Master Thesis/study/study3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2d319992da703ee6/Desktop/Master Thesis/master_thesis/study3/survey_materials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="319" documentId="8_{F03E348C-484E-4851-B57F-C9C00296541F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7DB31C04-E8D8-43BA-A691-12F0F379C360}"/>
+  <xr:revisionPtr revIDLastSave="329" documentId="8_{F03E348C-484E-4851-B57F-C9C00296541F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5E1D96D4-63E8-495A-B5E2-6E0E894DD793}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{847DDD94-B92E-45D0-A51E-EA1A53EC73AD}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{847DDD94-B92E-45D0-A51E-EA1A53EC73AD}"/>
   </bookViews>
   <sheets>
     <sheet name="ads" sheetId="4" r:id="rId1"/>
@@ -1775,10 +1775,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{248FE40E-FFA4-4659-9FF4-EC14E0C8AEA9}">
-  <dimension ref="B2:J12"/>
+  <dimension ref="B2:M12"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="L1" sqref="L1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.5"/>
@@ -1796,7 +1796,7 @@
     <col min="11" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" ht="20">
+    <row r="2" spans="2:13" ht="20">
       <c r="D2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1812,7 +1812,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="2:10" ht="150" customHeight="1">
+    <row r="3" spans="2:13" ht="150" customHeight="1">
       <c r="B3" s="5" t="s">
         <v>24</v>
       </c>
@@ -1830,8 +1830,16 @@
       <c r="J3" s="12" t="s">
         <v>25</v>
       </c>
+      <c r="L3" s="1">
+        <f>LEN(TRIM(D3))-LEN(SUBSTITUTE(D3," ",""))+1</f>
+        <v>37</v>
+      </c>
+      <c r="M3" s="1">
+        <f>LEN(TRIM(F3))-LEN(SUBSTITUTE(F3," ",""))+1</f>
+        <v>39</v>
+      </c>
     </row>
-    <row r="5" spans="2:10">
+    <row r="5" spans="2:13">
       <c r="D5" s="2" t="s">
         <v>0</v>
       </c>
@@ -1841,7 +1849,7 @@
       </c>
       <c r="G5" s="7"/>
     </row>
-    <row r="6" spans="2:10" ht="150" customHeight="1">
+    <row r="6" spans="2:13" ht="150" customHeight="1">
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1860,8 +1868,16 @@
       <c r="J6" s="12" t="s">
         <v>26</v>
       </c>
+      <c r="L6" s="1">
+        <f>LEN(TRIM(D6))-LEN(SUBSTITUTE(D6," ",""))+1</f>
+        <v>44</v>
+      </c>
+      <c r="M6" s="1">
+        <f>LEN(TRIM(F6))-LEN(SUBSTITUTE(F6," ",""))+1</f>
+        <v>37</v>
+      </c>
     </row>
-    <row r="8" spans="2:10">
+    <row r="8" spans="2:13">
       <c r="D8" s="2" t="s">
         <v>0</v>
       </c>
@@ -1871,7 +1887,7 @@
       </c>
       <c r="G8" s="7"/>
     </row>
-    <row r="9" spans="2:10" ht="150" customHeight="1">
+    <row r="9" spans="2:13" ht="150" customHeight="1">
       <c r="B9" s="5" t="s">
         <v>27</v>
       </c>
@@ -1889,8 +1905,16 @@
       <c r="J9" s="12" t="s">
         <v>28</v>
       </c>
+      <c r="L9" s="1">
+        <f>LEN(TRIM(D9))-LEN(SUBSTITUTE(D9," ",""))+1</f>
+        <v>37</v>
+      </c>
+      <c r="M9" s="1">
+        <f>LEN(TRIM(F9))-LEN(SUBSTITUTE(F9," ",""))+1</f>
+        <v>48</v>
+      </c>
     </row>
-    <row r="11" spans="2:10">
+    <row r="11" spans="2:13">
       <c r="D11" s="2" t="s">
         <v>0</v>
       </c>
@@ -1900,7 +1924,7 @@
       </c>
       <c r="G11" s="7"/>
     </row>
-    <row r="12" spans="2:10" ht="150" customHeight="1">
+    <row r="12" spans="2:13" ht="150" customHeight="1">
       <c r="B12" s="1" t="s">
         <v>7</v>
       </c>
@@ -1918,6 +1942,14 @@
       </c>
       <c r="J12" s="12" t="s">
         <v>26</v>
+      </c>
+      <c r="L12" s="1">
+        <f>LEN(TRIM(D12))-LEN(SUBSTITUTE(D12," ",""))+1</f>
+        <v>45</v>
+      </c>
+      <c r="M12" s="1">
+        <f>LEN(TRIM(F12))-LEN(SUBSTITUTE(F12," ",""))+1</f>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1928,10 +1960,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F973A1D5-55F6-4894-B192-9928091E6F9E}">
-  <dimension ref="B2:J12"/>
+  <dimension ref="B2:M12"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3:M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.5"/>
@@ -1949,7 +1981,7 @@
     <col min="11" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10">
+    <row r="2" spans="2:13">
       <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1959,7 +1991,7 @@
       </c>
       <c r="G2" s="7"/>
     </row>
-    <row r="3" spans="2:10" ht="150" customHeight="1">
+    <row r="3" spans="2:13" ht="150" customHeight="1">
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1978,8 +2010,16 @@
       <c r="J3" s="12" t="s">
         <v>26</v>
       </c>
+      <c r="L3" s="1">
+        <f>LEN(TRIM(D3))-LEN(SUBSTITUTE(D3," ",""))+1</f>
+        <v>41</v>
+      </c>
+      <c r="M3" s="1">
+        <f>LEN(TRIM(F3))-LEN(SUBSTITUTE(F3," ",""))+1</f>
+        <v>46</v>
+      </c>
     </row>
-    <row r="5" spans="2:10">
+    <row r="5" spans="2:13">
       <c r="D5" s="2" t="s">
         <v>2</v>
       </c>
@@ -1989,7 +2029,7 @@
       </c>
       <c r="G5" s="7"/>
     </row>
-    <row r="6" spans="2:10" ht="150" customHeight="1">
+    <row r="6" spans="2:13" ht="150" customHeight="1">
       <c r="B6" s="5" t="s">
         <v>16</v>
       </c>
@@ -2007,8 +2047,16 @@
       <c r="J6" s="12" t="s">
         <v>17</v>
       </c>
+      <c r="L6" s="1">
+        <f>LEN(TRIM(D6))-LEN(SUBSTITUTE(D6," ",""))+1</f>
+        <v>46</v>
+      </c>
+      <c r="M6" s="1">
+        <f>LEN(TRIM(F6))-LEN(SUBSTITUTE(F6," ",""))+1</f>
+        <v>40</v>
+      </c>
     </row>
-    <row r="8" spans="2:10">
+    <row r="8" spans="2:13">
       <c r="D8" s="2" t="s">
         <v>2</v>
       </c>
@@ -2018,7 +2066,7 @@
       </c>
       <c r="G8" s="7"/>
     </row>
-    <row r="9" spans="2:10" ht="150" customHeight="1">
+    <row r="9" spans="2:13" ht="150" customHeight="1">
       <c r="B9" s="1" t="s">
         <v>6</v>
       </c>
@@ -2037,8 +2085,16 @@
       <c r="J9" s="12" t="s">
         <v>26</v>
       </c>
+      <c r="L9" s="1">
+        <f>LEN(TRIM(D9))-LEN(SUBSTITUTE(D9," ",""))+1</f>
+        <v>47</v>
+      </c>
+      <c r="M9" s="1">
+        <f>LEN(TRIM(F9))-LEN(SUBSTITUTE(F9," ",""))+1</f>
+        <v>46</v>
+      </c>
     </row>
-    <row r="11" spans="2:10">
+    <row r="11" spans="2:13">
       <c r="D11" s="2" t="s">
         <v>2</v>
       </c>
@@ -2048,7 +2104,7 @@
       </c>
       <c r="G11" s="7"/>
     </row>
-    <row r="12" spans="2:10" ht="150" customHeight="1">
+    <row r="12" spans="2:13" ht="150" customHeight="1">
       <c r="B12" s="5" t="s">
         <v>18</v>
       </c>
@@ -2065,6 +2121,14 @@
       </c>
       <c r="J12" s="12" t="s">
         <v>19</v>
+      </c>
+      <c r="L12" s="1">
+        <f>LEN(TRIM(D12))-LEN(SUBSTITUTE(D12," ",""))+1</f>
+        <v>46</v>
+      </c>
+      <c r="M12" s="1">
+        <f>LEN(TRIM(F12))-LEN(SUBSTITUTE(F12," ",""))+1</f>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -2096,7 +2160,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61C16B58-02A0-4535-B7F0-74930D615BC4}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
       <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>

</xml_diff>